<commit_message>
remove whitespace from spreadsheet titles
</commit_message>
<xml_diff>
--- a/cms/metrics_documentation/data_migration/source_data/metrics_definitions_migration_edit.xlsx
+++ b/cms/metrics_documentation/data_migration/source_data/metrics_definitions_migration_edit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipstanley/Documents/projects/UKHSA/winter-pressures/winter-pressures-api/cms/metrics_documentation/data_migration/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipstanley/Documents/projects/UKHSA/winter-pressures/winter-pressures-api/cms/metrics_documentation/data_migration/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880EA4A1-33C9-F04C-8BCD-CCCFF055EE64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829E4435-8B15-E240-97CC-498A3CC392E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8920" yWindow="660" windowWidth="57900" windowHeight="22600" xr2:uid="{761B9231-95BC-4CC1-BF4F-419CF0B37169}"/>
+    <workbookView xWindow="23800" yWindow="600" windowWidth="42180" windowHeight="19340" xr2:uid="{761B9231-95BC-4CC1-BF4F-419CF0B37169}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,9 +116,6 @@
 A change from a number greater than 0 to 0 will be displayed as -100% i.e. a 100% decrease</t>
   </si>
   <si>
-    <t>COVID-19_cases_casesByDay</t>
-  </si>
-  <si>
     <t xml:space="preserve">This metric shows the number of reported new cases for each day. 
 New cases are reported by specimen date - the date the first sample that identified the infection was taken from an individual.
 </t>
@@ -149,9 +146,6 @@
 People who test positive again after a given time period are counted as new cases. In England people are counted as new cases if they test positive again more than 90 days after their last positive test. 
 Data for the last 5 days by specimen date are considered incomplete as it takes time to get test results and record them on relevant lab systems. Cases data for England includes all positive lab-confirmed PCR test results plus, positive rapid lateral flow tests unless followed by a negative PCR test taken within 72 hours.
 The value shown on a given date is the total of the reported new cases in the 7 days up to and including that date divided by 7.</t>
-  </si>
-  <si>
-    <t>COVID-19_cases_rateRollingMean</t>
   </si>
   <si>
     <t>This metric shows the rate per 100,000 people of reported new cases in the 7-day period ending on the dates shown. 
@@ -1008,18 +1002,9 @@
     <t>Healthcare admission rolling mean</t>
   </si>
   <si>
-    <t>Healthcare Occupied beds by day</t>
-  </si>
-  <si>
     <t>Headline tests 7 day total</t>
   </si>
   <si>
-    <t>Headline tests 7 day change</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Headline tests 7 day percent change</t>
-  </si>
-  <si>
     <t>Testing PCR count by day</t>
   </si>
   <si>
@@ -1032,15 +1017,9 @@
     <t>Headline vaccines autumn 23 uptake</t>
   </si>
   <si>
-    <t>vaccinations autumn 23 doses by day</t>
-  </si>
-  <si>
     <t>Vaccinations autumn 23 uptake by day</t>
   </si>
   <si>
-    <t>headline vaccines spring 23 uptake</t>
-  </si>
-  <si>
     <t>Vaccinations spring 23 doses by day</t>
   </si>
   <si>
@@ -1098,9 +1077,6 @@
     <t>This metric shows the rate per 100,000 people of reported new cases in the 7-day period ending on the dates shown.</t>
   </si>
   <si>
-    <t>his metric shows the total number of deaths in the last 7 days of people whose death certificate mentioned COVID-19 as one of the causes.</t>
-  </si>
-  <si>
     <t>This metric shows the difference between the total number of deaths in the last 7 days of people whose death certificate mentioned COVID-19 as one of the causes compared to the previous 7 days.</t>
   </si>
   <si>
@@ -1189,6 +1165,30 @@
   </si>
   <si>
     <t>This metric shows the percentage of the total number of PCR tests for RSV taken in the 7 days up to and including the date shown which had a positive result.</t>
+  </si>
+  <si>
+    <t>Headline tests 7 day percent change</t>
+  </si>
+  <si>
+    <t>COVID-19_cas+B7es_rateRollingMean</t>
+  </si>
+  <si>
+    <t>Cases cases +B7by day</t>
+  </si>
+  <si>
+    <t>Vaccinations autumn 23 doses by day</t>
+  </si>
+  <si>
+    <t>Headline vaccines spring 23 total</t>
+  </si>
+  <si>
+    <t>Headline vaccines spring 23 uptake</t>
+  </si>
+  <si>
+    <t>This metric shows the total number of deaths in the last 7 days of people whose death certificate mentioned COVID-19 as one of the causes.</t>
+  </si>
+  <si>
+    <t>Healthcare occupied beds by day</t>
   </si>
 </sst>
 </file>
@@ -1706,10 +1706,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2010,10 +2006,10 @@
   <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:C1048576"/>
+      <selection pane="bottomRight" activeCell="A43" sqref="A42:A43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2029,7 +2025,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2041,7 +2037,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -2052,7 +2048,7 @@
     </row>
     <row r="2" spans="1:7" ht="296" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>5</v>
@@ -2064,7 +2060,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>8</v>
@@ -2075,7 +2071,7 @@
     </row>
     <row r="3" spans="1:7" ht="255.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>10</v>
@@ -2087,7 +2083,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>12</v>
@@ -2098,7 +2094,7 @@
     </row>
     <row r="4" spans="1:7" ht="322.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>14</v>
@@ -2110,7 +2106,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>16</v>
@@ -2121,1163 +2117,1155 @@
     </row>
     <row r="5" spans="1:7" ht="257.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>18</v>
+        <v>269</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="F5" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="F5" s="8" t="s">
+      <c r="G5" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="304" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="F6" s="8" t="s">
-        <v>24</v>
-      </c>
       <c r="G6" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="304" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>25</v>
+        <v>268</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="237.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B8" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="E8" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="F8" s="14" t="s">
         <v>29</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>244</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>31</v>
       </c>
       <c r="G8" s="15"/>
     </row>
     <row r="9" spans="1:7" ht="254.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="E9" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>33</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>245</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>35</v>
       </c>
       <c r="G9" s="14"/>
     </row>
     <row r="10" spans="1:7" ht="274.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>238</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D10" s="13" t="s">
+      <c r="G10" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>246</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="202.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B11" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>239</v>
+      </c>
+      <c r="F11" s="14" t="s">
         <v>40</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>247</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>42</v>
       </c>
       <c r="G11" s="14"/>
     </row>
     <row r="12" spans="1:7" ht="244.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="B12" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>43</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D12" s="19" t="s">
-        <v>44</v>
-      </c>
-      <c r="E12" s="19" t="s">
-        <v>248</v>
-      </c>
-      <c r="F12" s="20" t="s">
-        <v>45</v>
       </c>
       <c r="G12" s="20"/>
     </row>
     <row r="13" spans="1:7" ht="244.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B13" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="F13" s="14" t="s">
         <v>46</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="F13" s="14" t="s">
-        <v>48</v>
       </c>
       <c r="G13" s="14"/>
     </row>
     <row r="14" spans="1:7" ht="138.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B14" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D14" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="E14" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" s="23" t="s">
         <v>50</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="23" t="s">
-        <v>52</v>
       </c>
       <c r="G14" s="24"/>
     </row>
     <row r="15" spans="1:7" ht="201" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="B15" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D15" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="F15" s="26" t="s">
         <v>53</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="25" t="s">
-        <v>250</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>55</v>
       </c>
       <c r="G15" s="25"/>
     </row>
     <row r="16" spans="1:7" ht="208.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B16" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="27" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="25" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="27" t="s">
-        <v>58</v>
-      </c>
       <c r="G16" s="28" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B17" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" s="25" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="29" t="s">
         <v>59</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="E17" s="25" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="29" t="s">
-        <v>61</v>
       </c>
       <c r="G17" s="30"/>
     </row>
     <row r="18" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B18" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="F18" s="29" t="s">
         <v>62</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D18" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="E18" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="29" t="s">
-        <v>64</v>
       </c>
       <c r="G18" s="30"/>
     </row>
     <row r="19" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B19" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F19" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D19" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>67</v>
-      </c>
       <c r="G19" s="31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="156.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B20" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="C20" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D20" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="33" t="s">
         <v>68</v>
-      </c>
-      <c r="C20" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D20" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="F20" s="33" t="s">
-        <v>70</v>
       </c>
       <c r="G20" s="34"/>
     </row>
     <row r="21" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B21" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="F21" s="35" t="s">
         <v>71</v>
-      </c>
-      <c r="C21" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="D21" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="E21" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="F21" s="35" t="s">
-        <v>73</v>
       </c>
       <c r="G21" s="36"/>
     </row>
     <row r="22" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>214</v>
+        <v>274</v>
       </c>
       <c r="B22" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="F22" s="37" t="s">
         <v>74</v>
-      </c>
-      <c r="C22" s="33" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="E22" s="25" t="s">
-        <v>75</v>
-      </c>
-      <c r="F22" s="37" t="s">
-        <v>76</v>
       </c>
       <c r="G22" s="36"/>
     </row>
     <row r="23" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A23" s="38" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B23" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="C23" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="C23" s="39" t="s">
+      <c r="E23" s="40" t="s">
+        <v>243</v>
+      </c>
+      <c r="F23" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="D23" s="40" t="s">
+      <c r="G23" s="42" t="s">
         <v>79</v>
-      </c>
-      <c r="E23" s="40" t="s">
-        <v>251</v>
-      </c>
-      <c r="F23" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="G23" s="42" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A24" s="38" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="B24" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="C24" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D24" s="43" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" s="55" t="s">
+        <v>244</v>
+      </c>
+      <c r="F24" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="C24" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="D24" s="43" t="s">
-        <v>83</v>
-      </c>
-      <c r="E24" s="55" t="s">
-        <v>252</v>
-      </c>
-      <c r="F24" s="41" t="s">
-        <v>84</v>
-      </c>
       <c r="G24" s="44" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A25" s="38" t="s">
-        <v>217</v>
+        <v>267</v>
       </c>
       <c r="B25" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="C25" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="E25" s="45" t="s">
+        <v>245</v>
+      </c>
+      <c r="F25" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="C25" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" s="45" t="s">
+      <c r="G25" s="44" t="s">
         <v>86</v>
-      </c>
-      <c r="E25" s="45" t="s">
-        <v>253</v>
-      </c>
-      <c r="F25" s="41" t="s">
-        <v>87</v>
-      </c>
-      <c r="G25" s="44" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A26" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="B26" s="38" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" s="46" t="s">
+        <v>88</v>
+      </c>
+      <c r="E26" s="46" t="s">
+        <v>246</v>
+      </c>
+      <c r="F26" s="41" t="s">
         <v>89</v>
       </c>
-      <c r="B26" s="38" t="s">
-        <v>89</v>
-      </c>
-      <c r="C26" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="D26" s="46" t="s">
-        <v>90</v>
-      </c>
-      <c r="E26" s="46" t="s">
-        <v>254</v>
-      </c>
-      <c r="F26" s="41" t="s">
-        <v>91</v>
-      </c>
       <c r="G26" s="44" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A27" s="38" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="B27" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="C27" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" s="40" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="40" t="s">
+        <v>247</v>
+      </c>
+      <c r="F27" s="41" t="s">
         <v>92</v>
       </c>
-      <c r="C27" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="D27" s="40" t="s">
-        <v>93</v>
-      </c>
-      <c r="E27" s="40" t="s">
-        <v>255</v>
-      </c>
-      <c r="F27" s="41" t="s">
-        <v>94</v>
-      </c>
       <c r="G27" s="44" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A28" s="38" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="B28" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="39" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="E28" s="46" t="s">
+        <v>248</v>
+      </c>
+      <c r="F28" s="41" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="46" t="s">
-        <v>96</v>
-      </c>
-      <c r="E28" s="46" t="s">
-        <v>256</v>
-      </c>
-      <c r="F28" s="41" t="s">
-        <v>97</v>
-      </c>
       <c r="G28" s="44" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A29" s="47" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B29" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="C29" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D29" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="C29" s="48" t="s">
+      <c r="E29" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="F29" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="D29" s="49" t="s">
+      <c r="G29" s="49" t="s">
         <v>100</v>
-      </c>
-      <c r="E29" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="F29" s="49" t="s">
-        <v>101</v>
-      </c>
-      <c r="G29" s="49" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A30" s="47" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="B30" s="47" t="s">
+        <v>101</v>
+      </c>
+      <c r="C30" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D30" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="E30" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="C30" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="D30" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="E30" s="49" t="s">
-        <v>104</v>
-      </c>
-      <c r="F30" s="49" t="s">
-        <v>105</v>
-      </c>
       <c r="G30" s="49" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A31" s="47" t="s">
-        <v>222</v>
+        <v>270</v>
       </c>
       <c r="B31" s="47" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D31" s="49" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" s="49" t="s">
+        <v>249</v>
+      </c>
+      <c r="F31" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="C31" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="D31" s="49" t="s">
-        <v>107</v>
-      </c>
-      <c r="E31" s="49" t="s">
-        <v>257</v>
-      </c>
-      <c r="F31" s="49" t="s">
-        <v>108</v>
-      </c>
       <c r="G31" s="49" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A32" s="47" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B32" s="47" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D32" s="49" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" s="49" t="s">
+        <v>250</v>
+      </c>
+      <c r="F32" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="C32" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="D32" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="E32" s="49" t="s">
-        <v>258</v>
-      </c>
-      <c r="F32" s="49" t="s">
-        <v>111</v>
-      </c>
       <c r="G32" s="49" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A33" s="47" t="s">
+        <v>271</v>
+      </c>
+      <c r="B33" s="47" t="s">
+        <v>110</v>
+      </c>
+      <c r="C33" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="E33" s="49" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="B33" s="47" t="s">
-        <v>112</v>
-      </c>
-      <c r="C33" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="D33" s="49" t="s">
+      <c r="G33" s="49" t="s">
         <v>113</v>
-      </c>
-      <c r="E33" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="F33" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="G33" s="49" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A34" s="47" t="s">
-        <v>224</v>
+        <v>272</v>
       </c>
       <c r="B34" s="47" t="s">
+        <v>114</v>
+      </c>
+      <c r="C34" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D34" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="E34" s="49" t="s">
+        <v>115</v>
+      </c>
+      <c r="F34" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="C34" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="D34" s="49" t="s">
-        <v>117</v>
-      </c>
-      <c r="E34" s="49" t="s">
-        <v>117</v>
-      </c>
-      <c r="F34" s="49" t="s">
-        <v>118</v>
-      </c>
       <c r="G34" s="49" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A35" s="47" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
       <c r="B35" s="47" t="s">
+        <v>117</v>
+      </c>
+      <c r="C35" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="49" t="s">
+        <v>118</v>
+      </c>
+      <c r="E35" s="49" t="s">
+        <v>251</v>
+      </c>
+      <c r="F35" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="C35" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="D35" s="49" t="s">
-        <v>120</v>
-      </c>
-      <c r="E35" s="49" t="s">
-        <v>259</v>
-      </c>
-      <c r="F35" s="49" t="s">
-        <v>121</v>
-      </c>
       <c r="G35" s="49" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A36" s="47" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="B36" s="47" t="s">
+        <v>120</v>
+      </c>
+      <c r="C36" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D36" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="E36" s="49" t="s">
+        <v>252</v>
+      </c>
+      <c r="F36" s="49" t="s">
         <v>122</v>
       </c>
-      <c r="C36" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" s="49" t="s">
-        <v>123</v>
-      </c>
-      <c r="E36" s="49" t="s">
-        <v>260</v>
-      </c>
-      <c r="F36" s="49" t="s">
-        <v>124</v>
-      </c>
       <c r="G36" s="49" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A37" s="47" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="B37" s="47" t="s">
+        <v>123</v>
+      </c>
+      <c r="C37" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" s="49" t="s">
+        <v>124</v>
+      </c>
+      <c r="E37" s="49" t="s">
+        <v>253</v>
+      </c>
+      <c r="F37" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="C37" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="D37" s="49" t="s">
+      <c r="G37" s="49" t="s">
         <v>126</v>
-      </c>
-      <c r="E37" s="49" t="s">
-        <v>261</v>
-      </c>
-      <c r="F37" s="49" t="s">
-        <v>127</v>
-      </c>
-      <c r="G37" s="49" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A38" s="47" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B38" s="47" t="s">
+        <v>127</v>
+      </c>
+      <c r="C38" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D38" s="49" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" s="49" t="s">
+        <v>254</v>
+      </c>
+      <c r="F38" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="C38" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="D38" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="E38" s="49" t="s">
-        <v>262</v>
-      </c>
-      <c r="F38" s="49" t="s">
-        <v>131</v>
-      </c>
       <c r="G38" s="49" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="272" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="B39" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="D39" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="C39" s="23" t="s">
+      <c r="E39" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="F39" s="26" t="s">
         <v>133</v>
       </c>
-      <c r="D39" s="25" t="s">
+      <c r="G39" s="25" t="s">
         <v>134</v>
-      </c>
-      <c r="E39" s="25" t="s">
-        <v>134</v>
-      </c>
-      <c r="F39" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="G39" s="25" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="272" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B40" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="F40" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="C40" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="D40" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="E40" s="25" t="s">
-        <v>138</v>
-      </c>
-      <c r="F40" s="26" t="s">
-        <v>139</v>
-      </c>
       <c r="G40" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="272" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="B41" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="E41" s="25" t="s">
+        <v>139</v>
+      </c>
+      <c r="F41" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C41" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="D41" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="E41" s="25" t="s">
-        <v>141</v>
-      </c>
-      <c r="F41" s="26" t="s">
-        <v>142</v>
-      </c>
       <c r="G41" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="272" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="B42" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>142</v>
+      </c>
+      <c r="F42" s="26" t="s">
         <v>143</v>
       </c>
-      <c r="C42" s="23" t="s">
-        <v>133</v>
-      </c>
-      <c r="D42" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="E42" s="25" t="s">
-        <v>144</v>
-      </c>
-      <c r="F42" s="26" t="s">
-        <v>145</v>
-      </c>
       <c r="G42" s="25" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A43" s="38" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B43" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="C43" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="D43" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="E43" s="46" t="s">
+        <v>255</v>
+      </c>
+      <c r="F43" s="41" t="s">
         <v>147</v>
-      </c>
-      <c r="D43" s="46" t="s">
-        <v>148</v>
-      </c>
-      <c r="E43" s="46" t="s">
-        <v>263</v>
-      </c>
-      <c r="F43" s="41" t="s">
-        <v>149</v>
       </c>
       <c r="G43" s="44"/>
     </row>
     <row r="44" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A44" s="38" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B44" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="C44" s="39" t="s">
+        <v>145</v>
+      </c>
+      <c r="D44" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="E44" s="46" t="s">
+        <v>256</v>
+      </c>
+      <c r="F44" s="41" t="s">
         <v>150</v>
-      </c>
-      <c r="C44" s="39" t="s">
-        <v>147</v>
-      </c>
-      <c r="D44" s="46" t="s">
-        <v>151</v>
-      </c>
-      <c r="E44" s="46" t="s">
-        <v>264</v>
-      </c>
-      <c r="F44" s="41" t="s">
-        <v>152</v>
       </c>
       <c r="G44" s="44"/>
     </row>
     <row r="45" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="B45" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="C45" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="E45" s="25" t="s">
+        <v>152</v>
+      </c>
+      <c r="F45" s="26" t="s">
         <v>153</v>
-      </c>
-      <c r="C45" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="D45" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="E45" s="25" t="s">
-        <v>154</v>
-      </c>
-      <c r="F45" s="26" t="s">
-        <v>155</v>
       </c>
       <c r="G45" s="36"/>
     </row>
     <row r="46" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="B46" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="C46" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="E46" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="F46" s="26" t="s">
         <v>156</v>
-      </c>
-      <c r="C46" s="50" t="s">
-        <v>50</v>
-      </c>
-      <c r="D46" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="E46" s="25" t="s">
-        <v>157</v>
-      </c>
-      <c r="F46" s="26" t="s">
-        <v>158</v>
       </c>
       <c r="G46" s="36"/>
     </row>
     <row r="47" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A47" s="51" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B47" s="51" t="s">
+        <v>157</v>
+      </c>
+      <c r="C47" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="D47" s="46" t="s">
         <v>159</v>
       </c>
-      <c r="C47" s="52" t="s">
+      <c r="E47" s="46" t="s">
+        <v>257</v>
+      </c>
+      <c r="F47" s="41" t="s">
         <v>160</v>
-      </c>
-      <c r="D47" s="46" t="s">
-        <v>161</v>
-      </c>
-      <c r="E47" s="46" t="s">
-        <v>265</v>
-      </c>
-      <c r="F47" s="41" t="s">
-        <v>162</v>
       </c>
       <c r="G47" s="53"/>
     </row>
     <row r="48" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A48" s="51" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B48" s="51" t="s">
+        <v>161</v>
+      </c>
+      <c r="C48" s="52" t="s">
+        <v>158</v>
+      </c>
+      <c r="D48" s="46" t="s">
+        <v>162</v>
+      </c>
+      <c r="E48" s="46" t="s">
+        <v>258</v>
+      </c>
+      <c r="F48" s="41" t="s">
         <v>163</v>
-      </c>
-      <c r="C48" s="52" t="s">
-        <v>160</v>
-      </c>
-      <c r="D48" s="46" t="s">
-        <v>164</v>
-      </c>
-      <c r="E48" s="46" t="s">
-        <v>266</v>
-      </c>
-      <c r="F48" s="41" t="s">
-        <v>165</v>
       </c>
       <c r="G48" s="53"/>
     </row>
     <row r="49" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A49" s="51" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B49" s="51" t="s">
+        <v>164</v>
+      </c>
+      <c r="C49" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="D49" s="46" t="s">
         <v>166</v>
       </c>
-      <c r="C49" s="52" t="s">
+      <c r="E49" s="46" t="s">
+        <v>259</v>
+      </c>
+      <c r="F49" s="41" t="s">
         <v>167</v>
-      </c>
-      <c r="D49" s="46" t="s">
-        <v>168</v>
-      </c>
-      <c r="E49" s="46" t="s">
-        <v>267</v>
-      </c>
-      <c r="F49" s="41" t="s">
-        <v>169</v>
       </c>
       <c r="G49" s="53"/>
     </row>
     <row r="50" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A50" s="51" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B50" s="51" t="s">
+        <v>168</v>
+      </c>
+      <c r="C50" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="D50" s="46" t="s">
+        <v>169</v>
+      </c>
+      <c r="E50" s="46" t="s">
+        <v>260</v>
+      </c>
+      <c r="F50" s="41" t="s">
         <v>170</v>
-      </c>
-      <c r="C50" s="52" t="s">
-        <v>167</v>
-      </c>
-      <c r="D50" s="46" t="s">
-        <v>171</v>
-      </c>
-      <c r="E50" s="46" t="s">
-        <v>268</v>
-      </c>
-      <c r="F50" s="41" t="s">
-        <v>172</v>
       </c>
       <c r="G50" s="53"/>
     </row>
     <row r="51" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A51" s="51" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B51" s="51" t="s">
+        <v>171</v>
+      </c>
+      <c r="C51" s="52" t="s">
+        <v>172</v>
+      </c>
+      <c r="D51" s="46" t="s">
         <v>173</v>
       </c>
-      <c r="C51" s="52" t="s">
+      <c r="E51" s="46" t="s">
+        <v>261</v>
+      </c>
+      <c r="F51" s="41" t="s">
         <v>174</v>
-      </c>
-      <c r="D51" s="46" t="s">
-        <v>175</v>
-      </c>
-      <c r="E51" s="46" t="s">
-        <v>269</v>
-      </c>
-      <c r="F51" s="41" t="s">
-        <v>176</v>
       </c>
       <c r="G51" s="53"/>
     </row>
     <row r="52" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A52" s="51" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B52" s="51" t="s">
+        <v>175</v>
+      </c>
+      <c r="C52" s="52" t="s">
+        <v>172</v>
+      </c>
+      <c r="D52" s="46" t="s">
+        <v>176</v>
+      </c>
+      <c r="E52" s="46" t="s">
+        <v>262</v>
+      </c>
+      <c r="F52" s="41" t="s">
         <v>177</v>
-      </c>
-      <c r="C52" s="52" t="s">
-        <v>174</v>
-      </c>
-      <c r="D52" s="46" t="s">
-        <v>178</v>
-      </c>
-      <c r="E52" s="46" t="s">
-        <v>270</v>
-      </c>
-      <c r="F52" s="41" t="s">
-        <v>179</v>
       </c>
       <c r="G52" s="53"/>
     </row>
     <row r="53" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A53" s="51" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B53" s="51" t="s">
+        <v>178</v>
+      </c>
+      <c r="C53" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="D53" s="46" t="s">
         <v>180</v>
       </c>
-      <c r="C53" s="52" t="s">
+      <c r="E53" s="46" t="s">
+        <v>263</v>
+      </c>
+      <c r="F53" s="41" t="s">
         <v>181</v>
-      </c>
-      <c r="D53" s="46" t="s">
-        <v>182</v>
-      </c>
-      <c r="E53" s="46" t="s">
-        <v>271</v>
-      </c>
-      <c r="F53" s="41" t="s">
-        <v>183</v>
       </c>
       <c r="G53" s="53"/>
     </row>
     <row r="54" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A54" s="51" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B54" s="51" t="s">
+        <v>182</v>
+      </c>
+      <c r="C54" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="D54" s="46" t="s">
+        <v>183</v>
+      </c>
+      <c r="E54" s="46" t="s">
+        <v>264</v>
+      </c>
+      <c r="F54" s="41" t="s">
         <v>184</v>
-      </c>
-      <c r="C54" s="52" t="s">
-        <v>181</v>
-      </c>
-      <c r="D54" s="46" t="s">
-        <v>185</v>
-      </c>
-      <c r="E54" s="46" t="s">
-        <v>272</v>
-      </c>
-      <c r="F54" s="41" t="s">
-        <v>186</v>
       </c>
       <c r="G54" s="53"/>
     </row>
     <row r="55" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A55" s="51" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="B55" s="51" t="s">
+        <v>185</v>
+      </c>
+      <c r="C55" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="D55" s="46" t="s">
         <v>187</v>
       </c>
-      <c r="C55" s="52" t="s">
+      <c r="E55" s="46" t="s">
+        <v>265</v>
+      </c>
+      <c r="F55" s="41" t="s">
         <v>188</v>
-      </c>
-      <c r="D55" s="46" t="s">
-        <v>189</v>
-      </c>
-      <c r="E55" s="46" t="s">
-        <v>273</v>
-      </c>
-      <c r="F55" s="41" t="s">
-        <v>190</v>
       </c>
       <c r="G55" s="53"/>
     </row>
     <row r="56" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A56" s="51" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="B56" s="51" t="s">
+        <v>189</v>
+      </c>
+      <c r="C56" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="D56" s="46" t="s">
+        <v>190</v>
+      </c>
+      <c r="E56" s="46" t="s">
+        <v>266</v>
+      </c>
+      <c r="F56" s="41" t="s">
         <v>191</v>
-      </c>
-      <c r="C56" s="52" t="s">
-        <v>188</v>
-      </c>
-      <c r="D56" s="46" t="s">
-        <v>192</v>
-      </c>
-      <c r="E56" s="46" t="s">
-        <v>274</v>
-      </c>
-      <c r="F56" s="41" t="s">
-        <v>193</v>
       </c>
       <c r="G56" s="53"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B083713AC7608747A82F5A763B7281ED" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="427dd16ae52d8d155578e7a775f968a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3b0c4c8b-09b7-4186-9978-0ad6f7aa3547" xmlns:ns3="42387920-875b-4eae-aa9b-06edaadfbbd9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="154d5f4f1df4d06a6441f4dc4f97264b" ns2:_="" ns3:_="">
     <xsd:import namespace="3b0c4c8b-09b7-4186-9978-0ad6f7aa3547"/>
@@ -3500,7 +3488,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="3b0c4c8b-09b7-4186-9978-0ad6f7aa3547">
@@ -3511,15 +3499,16 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3CD4AA4-09C8-4CFA-BB33-8F852CC5F422}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C75314D-5D32-4004-AEB1-819C7303AD9A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3538,7 +3527,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF8AB170-7F52-477D-A194-577DDB38F42D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -3547,4 +3536,12 @@
     <ds:schemaRef ds:uri="42387920-875b-4eae-aa9b-06edaadfbbd9"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3CD4AA4-09C8-4CFA-BB33-8F852CC5F422}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add seo_title and search description
</commit_message>
<xml_diff>
--- a/cms/metrics_documentation/data_migration/source_data/metrics_definitions_migration_edit.xlsx
+++ b/cms/metrics_documentation/data_migration/source_data/metrics_definitions_migration_edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipstanley/Documents/projects/UKHSA/winter-pressures/winter-pressures-api/cms/metrics_documentation/data_migration/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{829E4435-8B15-E240-97CC-498A3CC392E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD0A6AF-8F08-E14A-BE18-23A43312A04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23800" yWindow="600" windowWidth="42180" windowHeight="19340" xr2:uid="{761B9231-95BC-4CC1-BF4F-419CF0B37169}"/>
+    <workbookView xWindow="940" yWindow="580" windowWidth="21920" windowHeight="24940" xr2:uid="{761B9231-95BC-4CC1-BF4F-419CF0B37169}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1170,12 +1170,6 @@
     <t>Headline tests 7 day percent change</t>
   </si>
   <si>
-    <t>COVID-19_cas+B7es_rateRollingMean</t>
-  </si>
-  <si>
-    <t>Cases cases +B7by day</t>
-  </si>
-  <si>
     <t>Vaccinations autumn 23 doses by day</t>
   </si>
   <si>
@@ -1189,6 +1183,12 @@
   </si>
   <si>
     <t>Healthcare occupied beds by day</t>
+  </si>
+  <si>
+    <t>COVID-19_cases_rateRollingMean</t>
+  </si>
+  <si>
+    <t>COVID-19_cases_casesByDay</t>
   </si>
 </sst>
 </file>
@@ -2006,10 +2006,10 @@
   <dimension ref="A1:G56"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C45" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A43" sqref="A42:A43"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2120,7 +2120,7 @@
         <v>204</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>269</v>
+        <v>274</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>6</v>
@@ -2166,7 +2166,7 @@
         <v>202</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>6</v>
@@ -2198,7 +2198,7 @@
         <v>28</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>29</v>
@@ -2486,7 +2486,7 @@
     </row>
     <row r="22" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B22" s="32" t="s">
         <v>72</v>
@@ -2691,7 +2691,7 @@
     </row>
     <row r="31" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A31" s="47" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B31" s="47" t="s">
         <v>104</v>
@@ -2737,7 +2737,7 @@
     </row>
     <row r="33" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A33" s="47" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B33" s="47" t="s">
         <v>110</v>
@@ -2760,7 +2760,7 @@
     </row>
     <row r="34" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A34" s="47" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B34" s="47" t="s">
         <v>114</v>
@@ -3266,6 +3266,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3b0c4c8b-09b7-4186-9978-0ad6f7aa3547">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42387920-875b-4eae-aa9b-06edaadfbbd9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B083713AC7608747A82F5A763B7281ED" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="427dd16ae52d8d155578e7a775f968a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3b0c4c8b-09b7-4186-9978-0ad6f7aa3547" xmlns:ns3="42387920-875b-4eae-aa9b-06edaadfbbd9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="154d5f4f1df4d06a6441f4dc4f97264b" ns2:_="" ns3:_="">
     <xsd:import namespace="3b0c4c8b-09b7-4186-9978-0ad6f7aa3547"/>
@@ -3488,27 +3508,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3b0c4c8b-09b7-4186-9978-0ad6f7aa3547">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42387920-875b-4eae-aa9b-06edaadfbbd9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3CD4AA4-09C8-4CFA-BB33-8F852CC5F422}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF8AB170-7F52-477D-A194-577DDB38F42D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3b0c4c8b-09b7-4186-9978-0ad6f7aa3547"/>
+    <ds:schemaRef ds:uri="42387920-875b-4eae-aa9b-06edaadfbbd9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C75314D-5D32-4004-AEB1-819C7303AD9A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3525,23 +3544,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FF8AB170-7F52-477D-A194-577DDB38F42D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3b0c4c8b-09b7-4186-9978-0ad6f7aa3547"/>
-    <ds:schemaRef ds:uri="42387920-875b-4eae-aa9b-06edaadfbbd9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3CD4AA4-09C8-4CFA-BB33-8F852CC5F422}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update titles in worksheet
</commit_message>
<xml_diff>
--- a/cms/metrics_documentation/data_migration/source_data/metrics_definitions_migration_edit.xlsx
+++ b/cms/metrics_documentation/data_migration/source_data/metrics_definitions_migration_edit.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phillipstanley/Documents/projects/UKHSA/winter-pressures/winter-pressures-api/cms/metrics_documentation/data_migration/source_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCD0A6AF-8F08-E14A-BE18-23A43312A04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CD4CBD6-20F5-4E4A-8B45-6BA6A24BE27B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="580" windowWidth="21920" windowHeight="24940" xr2:uid="{761B9231-95BC-4CC1-BF4F-419CF0B37169}"/>
+    <workbookView xWindow="24300" yWindow="1860" windowWidth="39240" windowHeight="24920" xr2:uid="{761B9231-95BC-4CC1-BF4F-419CF0B37169}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="284">
   <si>
     <t>Metric Name</t>
   </si>
@@ -516,9 +516,6 @@
     <t>Results from PCR tests only - LFD results are not included</t>
   </si>
   <si>
-    <t>COVID-19_headline_tests_7DayChange</t>
-  </si>
-  <si>
     <t>This metric shows the difference in the count of new positive and negative COVID-19 test results taken in the last 7 days compared to the previous 7 days.  
 Data is shown by the date that the test was taken (specimen date).</t>
   </si>
@@ -649,9 +646,6 @@
 People who are eligible for an spring booster vaccination but are less than 75 years old (e.g. immunocompromised individuals) are not included in the count.</t>
   </si>
   <si>
-    <t>COVID-19_headline_vaccines_spring23Uptake</t>
-  </si>
-  <si>
     <t>This metric shows the uptake of vaccinations given as part of the spring booster campaign in 2023</t>
   </si>
   <si>
@@ -945,117 +939,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Headline 7 day occupied beds percent change</t>
-  </si>
-  <si>
-    <t>Headline 7 day occupied beds change</t>
-  </si>
-  <si>
-    <t>Headline 7 day admissions percent change</t>
-  </si>
-  <si>
-    <t>Headline 7 day admissions</t>
-  </si>
-  <si>
-    <t>Deaths ONS by week</t>
-  </si>
-  <si>
-    <t>Deaths ONS by day</t>
-  </si>
-  <si>
-    <t>Headline ONS deaths 7 day percent change</t>
-  </si>
-  <si>
-    <t>Headline ONS deaths 7 day change</t>
-  </si>
-  <si>
-    <t>Headline ONS deaths 7 day totals</t>
-  </si>
-  <si>
-    <t>Cases rate rolling mean</t>
-  </si>
-  <si>
-    <t>Cases count rolling mean</t>
-  </si>
-  <si>
-    <t>Cases cases by day</t>
-  </si>
-  <si>
-    <t>Headline cases 7 day percent change</t>
-  </si>
-  <si>
-    <t>Headline cases 7 day change</t>
-  </si>
-  <si>
-    <t>Headline cases 7 day totals</t>
-  </si>
-  <si>
-    <t>Headline 7 day admissions change</t>
-  </si>
-  <si>
-    <t>Headline7 day occupied beds</t>
-  </si>
-  <si>
-    <t>Healthcare admission by day</t>
-  </si>
-  <si>
-    <t>Healthcare admission rolling mean</t>
-  </si>
-  <si>
-    <t>Headline tests 7 day total</t>
-  </si>
-  <si>
-    <t>Testing PCR count by day</t>
-  </si>
-  <si>
-    <t>Testing positivity 7 day rolling</t>
-  </si>
-  <si>
-    <t>Headline vaccines autumn 23 total</t>
-  </si>
-  <si>
-    <t>Headline vaccines autumn 23 uptake</t>
-  </si>
-  <si>
-    <t>Vaccinations autumn 23 uptake by day</t>
-  </si>
-  <si>
-    <t>Vaccinations spring 23 doses by day</t>
-  </si>
-  <si>
-    <t>Vaccinations spring 23 uptake by day</t>
-  </si>
-  <si>
-    <t>Vaccinations autumn 22 doses by day</t>
-  </si>
-  <si>
-    <t>Vaccinations autumn 22 uptake by day</t>
-  </si>
-  <si>
-    <t>Headline ICUHDU admission rate latest</t>
-  </si>
-  <si>
-    <t>Headline ICUHDU admission rate change</t>
-  </si>
-  <si>
-    <t>Headline ICUHDU admission rate percent change</t>
-  </si>
-  <si>
-    <t>Healthcare ICUHDU admission rate by week</t>
-  </si>
-  <si>
-    <t>Headline positivity latest</t>
-  </si>
-  <si>
-    <t>Testing positivity by week</t>
-  </si>
-  <si>
-    <t>Headline admission rate latest</t>
-  </si>
-  <si>
-    <t>Healthcare admission rate by week</t>
-  </si>
-  <si>
     <t>This metric shows the count of reported new cases in the last 7 days.</t>
   </si>
   <si>
@@ -1167,28 +1050,172 @@
     <t>This metric shows the percentage of the total number of PCR tests for RSV taken in the 7 days up to and including the date shown which had a positive result.</t>
   </si>
   <si>
-    <t>Headline tests 7 day percent change</t>
-  </si>
-  <si>
-    <t>Vaccinations autumn 23 doses by day</t>
-  </si>
-  <si>
-    <t>Headline vaccines spring 23 total</t>
-  </si>
-  <si>
-    <t>Headline vaccines spring 23 uptake</t>
-  </si>
-  <si>
     <t>This metric shows the total number of deaths in the last 7 days of people whose death certificate mentioned COVID-19 as one of the causes.</t>
   </si>
   <si>
-    <t>Healthcare occupied beds by day</t>
-  </si>
-  <si>
     <t>COVID-19_cases_rateRollingMean</t>
   </si>
   <si>
     <t>COVID-19_cases_casesByDay</t>
+  </si>
+  <si>
+    <t>COVID-19 headline cases 7 day change</t>
+  </si>
+  <si>
+    <t>COVID-19 headline cases 7 day percent change</t>
+  </si>
+  <si>
+    <t>COVID-19 cases cases by day</t>
+  </si>
+  <si>
+    <t>COVID-19 cases count rolling mean</t>
+  </si>
+  <si>
+    <t>COVID-19 cases rate rolling mean</t>
+  </si>
+  <si>
+    <t>COVID-19 headline ONS deaths 7 day totals</t>
+  </si>
+  <si>
+    <t>COVID-19 headline ONS deaths 7 day change</t>
+  </si>
+  <si>
+    <t>COVID-19 headline ONS deaths 7 day percent change</t>
+  </si>
+  <si>
+    <t>COVID-19 deaths ONS by day</t>
+  </si>
+  <si>
+    <t>COVID-19 deaths ONS by week</t>
+  </si>
+  <si>
+    <t>COVID-19 headline 7 day admissions</t>
+  </si>
+  <si>
+    <t>COVID-19 headline 7 day admissions change</t>
+  </si>
+  <si>
+    <t>COVID-19 headline 7 day admissions percent change</t>
+  </si>
+  <si>
+    <t>COVID-19 headline7 day occupied beds</t>
+  </si>
+  <si>
+    <t>COVID-19 headline 7 day occupied beds change</t>
+  </si>
+  <si>
+    <t>COVID-19 headline 7 day occupied beds percent change</t>
+  </si>
+  <si>
+    <t>COVID-19 healthcare admission by day</t>
+  </si>
+  <si>
+    <t>COVID-19 healthcare admission rolling mean</t>
+  </si>
+  <si>
+    <t>COVID-19 healthcare occupied beds by day</t>
+  </si>
+  <si>
+    <t>COVID-19 headline tests 7 day total</t>
+  </si>
+  <si>
+    <t>COVID-19 headline positivity latest</t>
+  </si>
+  <si>
+    <t>COVID-19 testing PCR count by day</t>
+  </si>
+  <si>
+    <t>COVID-19 testing positivity 7 day rolling</t>
+  </si>
+  <si>
+    <t>COVID-19 headline vaccines autumn 23 total</t>
+  </si>
+  <si>
+    <t>COVID-19 headline vaccines autumn 23 uptake</t>
+  </si>
+  <si>
+    <t>COVID-19 vaccinations autumn 23 doses by day</t>
+  </si>
+  <si>
+    <t>COVID-19 vaccinations autumn 23 uptake by day</t>
+  </si>
+  <si>
+    <t>COVID-19 headline vaccines spring 23 total</t>
+  </si>
+  <si>
+    <t>COVID-19 headline vaccines spring 23 uptake</t>
+  </si>
+  <si>
+    <t>COVID-19 vaccinations spring 23 doses by day</t>
+  </si>
+  <si>
+    <t>COVID-19 vaccinations spring 23 uptake by day</t>
+  </si>
+  <si>
+    <t>COVID-19 vaccinations autumn 22 doses by day</t>
+  </si>
+  <si>
+    <t>COVID-19 vaccinations autumn 22 uptake by day</t>
+  </si>
+  <si>
+    <t>Influenza headline ICUHDU admission rate latest</t>
+  </si>
+  <si>
+    <t>Influenza headline ICUHDU admission rate change</t>
+  </si>
+  <si>
+    <t>Influenza headline ICUHDU admission rate percent change</t>
+  </si>
+  <si>
+    <t>Influenza healthcare ICUHDU admission rate by week</t>
+  </si>
+  <si>
+    <t>Influenza headline positivity latest</t>
+  </si>
+  <si>
+    <t>Influenza testing positivity by week</t>
+  </si>
+  <si>
+    <t>RSV headline admission rate latest</t>
+  </si>
+  <si>
+    <t>RSV healthcare admission rate by week</t>
+  </si>
+  <si>
+    <t>Adenovirus headline positivity latest</t>
+  </si>
+  <si>
+    <t>Adenovirus testing positivity by week</t>
+  </si>
+  <si>
+    <t>hMPV headline positivity latest</t>
+  </si>
+  <si>
+    <t>hMPV testing positivity by week</t>
+  </si>
+  <si>
+    <t>Parainfluenza headline positivity latest</t>
+  </si>
+  <si>
+    <t>Parainfluenza testing positivity by week</t>
+  </si>
+  <si>
+    <t>Rhinovirus headline positivity latest</t>
+  </si>
+  <si>
+    <t>Rhinovirus testing positivity by week</t>
+  </si>
+  <si>
+    <t>RSV headline positivity latest</t>
+  </si>
+  <si>
+    <t>RSV testing positivity by week</t>
+  </si>
+  <si>
+    <t>COVID-19 headline tests 7 day percent change</t>
+  </si>
+  <si>
+    <t>COVID-19 headline cases 7 day totals</t>
   </si>
 </sst>
 </file>
@@ -2005,11 +2032,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E3E244-777F-44C7-8F0C-8F9E73605F19}">
   <dimension ref="A1:G56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2025,7 +2052,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -2037,7 +2064,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>231</v>
+        <v>192</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
@@ -2048,7 +2075,7 @@
     </row>
     <row r="2" spans="1:7" ht="296" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>207</v>
+        <v>283</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>5</v>
@@ -2060,7 +2087,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>230</v>
+        <v>191</v>
       </c>
       <c r="F2" s="8" t="s">
         <v>8</v>
@@ -2071,7 +2098,7 @@
     </row>
     <row r="3" spans="1:7" ht="255.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>10</v>
@@ -2083,7 +2110,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>232</v>
+        <v>193</v>
       </c>
       <c r="F3" s="8" t="s">
         <v>12</v>
@@ -2094,7 +2121,7 @@
     </row>
     <row r="4" spans="1:7" ht="322.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>205</v>
+        <v>232</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>14</v>
@@ -2106,7 +2133,7 @@
         <v>15</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>233</v>
+        <v>194</v>
       </c>
       <c r="F4" s="8" t="s">
         <v>16</v>
@@ -2117,10 +2144,10 @@
     </row>
     <row r="5" spans="1:7" ht="257.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>204</v>
+        <v>233</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>274</v>
+        <v>230</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>6</v>
@@ -2129,7 +2156,7 @@
         <v>18</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>234</v>
+        <v>195</v>
       </c>
       <c r="F5" s="8" t="s">
         <v>19</v>
@@ -2140,7 +2167,7 @@
     </row>
     <row r="6" spans="1:7" ht="304" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9" t="s">
-        <v>203</v>
+        <v>234</v>
       </c>
       <c r="B6" s="9" t="s">
         <v>21</v>
@@ -2152,7 +2179,7 @@
         <v>22</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>235</v>
+        <v>196</v>
       </c>
       <c r="F6" s="8" t="s">
         <v>23</v>
@@ -2163,10 +2190,10 @@
     </row>
     <row r="7" spans="1:7" ht="304" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>202</v>
+        <v>235</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>273</v>
+        <v>229</v>
       </c>
       <c r="C7" s="7" t="s">
         <v>6</v>
@@ -2175,7 +2202,7 @@
         <v>24</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>236</v>
+        <v>197</v>
       </c>
       <c r="F7" s="8" t="s">
         <v>25</v>
@@ -2186,7 +2213,7 @@
     </row>
     <row r="8" spans="1:7" ht="237.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
-        <v>201</v>
+        <v>236</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>26</v>
@@ -2198,7 +2225,7 @@
         <v>28</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>271</v>
+        <v>228</v>
       </c>
       <c r="F8" s="14" t="s">
         <v>29</v>
@@ -2207,7 +2234,7 @@
     </row>
     <row r="9" spans="1:7" ht="254.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
-        <v>200</v>
+        <v>237</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>30</v>
@@ -2219,7 +2246,7 @@
         <v>32</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="F9" s="14" t="s">
         <v>33</v>
@@ -2228,7 +2255,7 @@
     </row>
     <row r="10" spans="1:7" ht="274.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>199</v>
+        <v>238</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>34</v>
@@ -2240,7 +2267,7 @@
         <v>35</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>238</v>
+        <v>199</v>
       </c>
       <c r="F10" s="14" t="s">
         <v>36</v>
@@ -2251,7 +2278,7 @@
     </row>
     <row r="11" spans="1:7" ht="202.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
-        <v>199</v>
+        <v>238</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>38</v>
@@ -2263,7 +2290,7 @@
         <v>39</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>239</v>
+        <v>200</v>
       </c>
       <c r="F11" s="14" t="s">
         <v>40</v>
@@ -2272,7 +2299,7 @@
     </row>
     <row r="12" spans="1:7" ht="244.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
-        <v>198</v>
+        <v>239</v>
       </c>
       <c r="B12" s="16" t="s">
         <v>41</v>
@@ -2284,7 +2311,7 @@
         <v>42</v>
       </c>
       <c r="E12" s="19" t="s">
-        <v>240</v>
+        <v>201</v>
       </c>
       <c r="F12" s="20" t="s">
         <v>43</v>
@@ -2293,7 +2320,7 @@
     </row>
     <row r="13" spans="1:7" ht="244.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="17" t="s">
-        <v>197</v>
+        <v>240</v>
       </c>
       <c r="B13" s="17" t="s">
         <v>44</v>
@@ -2305,7 +2332,7 @@
         <v>45</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>241</v>
+        <v>202</v>
       </c>
       <c r="F13" s="14" t="s">
         <v>46</v>
@@ -2314,7 +2341,7 @@
     </row>
     <row r="14" spans="1:7" ht="138.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
-        <v>196</v>
+        <v>241</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>47</v>
@@ -2335,7 +2362,7 @@
     </row>
     <row r="15" spans="1:7" ht="201" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
-        <v>208</v>
+        <v>242</v>
       </c>
       <c r="B15" s="21" t="s">
         <v>51</v>
@@ -2347,7 +2374,7 @@
         <v>52</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>242</v>
+        <v>203</v>
       </c>
       <c r="F15" s="26" t="s">
         <v>53</v>
@@ -2356,7 +2383,7 @@
     </row>
     <row r="16" spans="1:7" ht="208.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
-        <v>195</v>
+        <v>243</v>
       </c>
       <c r="B16" s="21" t="s">
         <v>54</v>
@@ -2379,7 +2406,7 @@
     </row>
     <row r="17" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
-        <v>209</v>
+        <v>244</v>
       </c>
       <c r="B17" s="22" t="s">
         <v>57</v>
@@ -2400,7 +2427,7 @@
     </row>
     <row r="18" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="B18" s="22" t="s">
         <v>60</v>
@@ -2421,7 +2448,7 @@
     </row>
     <row r="19" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A19" s="22" t="s">
-        <v>193</v>
+        <v>246</v>
       </c>
       <c r="B19" s="22" t="s">
         <v>63</v>
@@ -2444,7 +2471,7 @@
     </row>
     <row r="20" spans="1:7" ht="156.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
-        <v>210</v>
+        <v>247</v>
       </c>
       <c r="B20" s="32" t="s">
         <v>66</v>
@@ -2465,7 +2492,7 @@
     </row>
     <row r="21" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A21" s="22" t="s">
-        <v>211</v>
+        <v>248</v>
       </c>
       <c r="B21" s="22" t="s">
         <v>69</v>
@@ -2486,7 +2513,7 @@
     </row>
     <row r="22" spans="1:7" ht="96" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
       <c r="B22" s="32" t="s">
         <v>72</v>
@@ -2507,7 +2534,7 @@
     </row>
     <row r="23" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A23" s="38" t="s">
-        <v>212</v>
+        <v>250</v>
       </c>
       <c r="B23" s="38" t="s">
         <v>75</v>
@@ -2519,7 +2546,7 @@
         <v>77</v>
       </c>
       <c r="E23" s="40" t="s">
-        <v>243</v>
+        <v>204</v>
       </c>
       <c r="F23" s="41" t="s">
         <v>78</v>
@@ -2530,22 +2557,22 @@
     </row>
     <row r="24" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A24" s="38" t="s">
-        <v>212</v>
+        <v>250</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>80</v>
+        <v>250</v>
       </c>
       <c r="C24" s="39" t="s">
         <v>76</v>
       </c>
       <c r="D24" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="E24" s="55" t="s">
+        <v>205</v>
+      </c>
+      <c r="F24" s="41" t="s">
         <v>81</v>
-      </c>
-      <c r="E24" s="55" t="s">
-        <v>244</v>
-      </c>
-      <c r="F24" s="41" t="s">
-        <v>82</v>
       </c>
       <c r="G24" s="44" t="s">
         <v>79</v>
@@ -2553,45 +2580,45 @@
     </row>
     <row r="25" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A25" s="38" t="s">
-        <v>267</v>
+        <v>282</v>
       </c>
       <c r="B25" s="38" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C25" s="39" t="s">
         <v>76</v>
       </c>
       <c r="D25" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="F25" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="E25" s="45" t="s">
-        <v>245</v>
-      </c>
-      <c r="F25" s="41" t="s">
+      <c r="G25" s="44" t="s">
         <v>85</v>
-      </c>
-      <c r="G25" s="44" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A26" s="38" t="s">
-        <v>226</v>
+        <v>251</v>
       </c>
       <c r="B26" s="38" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C26" s="39" t="s">
         <v>76</v>
       </c>
       <c r="D26" s="46" t="s">
+        <v>87</v>
+      </c>
+      <c r="E26" s="46" t="s">
+        <v>207</v>
+      </c>
+      <c r="F26" s="41" t="s">
         <v>88</v>
-      </c>
-      <c r="E26" s="46" t="s">
-        <v>246</v>
-      </c>
-      <c r="F26" s="41" t="s">
-        <v>89</v>
       </c>
       <c r="G26" s="44" t="s">
         <v>79</v>
@@ -2599,22 +2626,22 @@
     </row>
     <row r="27" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A27" s="38" t="s">
-        <v>213</v>
+        <v>252</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C27" s="39" t="s">
         <v>76</v>
       </c>
       <c r="D27" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="E27" s="40" t="s">
+        <v>208</v>
+      </c>
+      <c r="F27" s="41" t="s">
         <v>91</v>
-      </c>
-      <c r="E27" s="40" t="s">
-        <v>247</v>
-      </c>
-      <c r="F27" s="41" t="s">
-        <v>92</v>
       </c>
       <c r="G27" s="44" t="s">
         <v>79</v>
@@ -2622,22 +2649,22 @@
     </row>
     <row r="28" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A28" s="38" t="s">
-        <v>214</v>
+        <v>253</v>
       </c>
       <c r="B28" s="38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C28" s="39" t="s">
         <v>76</v>
       </c>
       <c r="D28" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="E28" s="46" t="s">
+        <v>209</v>
+      </c>
+      <c r="F28" s="41" t="s">
         <v>94</v>
-      </c>
-      <c r="E28" s="46" t="s">
-        <v>248</v>
-      </c>
-      <c r="F28" s="41" t="s">
-        <v>95</v>
       </c>
       <c r="G28" s="44" t="s">
         <v>79</v>
@@ -2645,617 +2672,617 @@
     </row>
     <row r="29" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A29" s="47" t="s">
-        <v>215</v>
+        <v>254</v>
       </c>
       <c r="B29" s="47" t="s">
+        <v>95</v>
+      </c>
+      <c r="C29" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="C29" s="48" t="s">
+      <c r="D29" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="D29" s="49" t="s">
+      <c r="E29" s="49" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="E29" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="F29" s="49" t="s">
+      <c r="G29" s="49" t="s">
         <v>99</v>
-      </c>
-      <c r="G29" s="49" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A30" s="47" t="s">
-        <v>216</v>
+        <v>255</v>
       </c>
       <c r="B30" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="C30" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="D30" s="49" t="s">
+      <c r="E30" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="F30" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="E30" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="F30" s="49" t="s">
-        <v>103</v>
-      </c>
       <c r="G30" s="49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A31" s="47" t="s">
-        <v>268</v>
+        <v>256</v>
       </c>
       <c r="B31" s="47" t="s">
+        <v>103</v>
+      </c>
+      <c r="C31" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="D31" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="C31" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="D31" s="49" t="s">
+      <c r="E31" s="49" t="s">
+        <v>210</v>
+      </c>
+      <c r="F31" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="E31" s="49" t="s">
-        <v>249</v>
-      </c>
-      <c r="F31" s="49" t="s">
-        <v>106</v>
-      </c>
       <c r="G31" s="49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A32" s="47" t="s">
-        <v>217</v>
+        <v>257</v>
       </c>
       <c r="B32" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="C32" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="C32" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="D32" s="49" t="s">
+      <c r="E32" s="49" t="s">
+        <v>211</v>
+      </c>
+      <c r="F32" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="E32" s="49" t="s">
-        <v>250</v>
-      </c>
-      <c r="F32" s="49" t="s">
-        <v>109</v>
-      </c>
       <c r="G32" s="49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A33" s="47" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B33" s="47" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="D33" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="C33" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="D33" s="49" t="s">
+      <c r="E33" s="49" t="s">
+        <v>110</v>
+      </c>
+      <c r="F33" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="E33" s="49" t="s">
-        <v>111</v>
-      </c>
-      <c r="F33" s="49" t="s">
+      <c r="G33" s="49" t="s">
         <v>112</v>
-      </c>
-      <c r="G33" s="49" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A34" s="47" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="B34" s="47" t="s">
+        <v>260</v>
+      </c>
+      <c r="C34" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="D34" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34" s="49" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="C34" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="D34" s="49" t="s">
-        <v>115</v>
-      </c>
-      <c r="E34" s="49" t="s">
-        <v>115</v>
-      </c>
-      <c r="F34" s="49" t="s">
-        <v>116</v>
-      </c>
       <c r="G34" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A35" s="47" t="s">
-        <v>218</v>
+        <v>260</v>
       </c>
       <c r="B35" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="C35" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="49" t="s">
+        <v>116</v>
+      </c>
+      <c r="E35" s="49" t="s">
+        <v>212</v>
+      </c>
+      <c r="F35" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="C35" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="D35" s="49" t="s">
-        <v>118</v>
-      </c>
-      <c r="E35" s="49" t="s">
-        <v>251</v>
-      </c>
-      <c r="F35" s="49" t="s">
-        <v>119</v>
-      </c>
       <c r="G35" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A36" s="47" t="s">
-        <v>219</v>
+        <v>261</v>
       </c>
       <c r="B36" s="47" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="49" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" s="49" t="s">
+        <v>213</v>
+      </c>
+      <c r="F36" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="C36" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="D36" s="49" t="s">
-        <v>121</v>
-      </c>
-      <c r="E36" s="49" t="s">
-        <v>252</v>
-      </c>
-      <c r="F36" s="49" t="s">
-        <v>122</v>
-      </c>
       <c r="G36" s="49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="176" x14ac:dyDescent="0.2">
       <c r="A37" s="47" t="s">
-        <v>220</v>
+        <v>262</v>
       </c>
       <c r="B37" s="47" t="s">
+        <v>121</v>
+      </c>
+      <c r="C37" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="D37" s="49" t="s">
+        <v>122</v>
+      </c>
+      <c r="E37" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="F37" s="49" t="s">
         <v>123</v>
       </c>
-      <c r="C37" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="D37" s="49" t="s">
+      <c r="G37" s="49" t="s">
         <v>124</v>
-      </c>
-      <c r="E37" s="49" t="s">
-        <v>253</v>
-      </c>
-      <c r="F37" s="49" t="s">
-        <v>125</v>
-      </c>
-      <c r="G37" s="49" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="192" x14ac:dyDescent="0.2">
       <c r="A38" s="47" t="s">
-        <v>221</v>
+        <v>263</v>
       </c>
       <c r="B38" s="47" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="D38" s="49" t="s">
+        <v>126</v>
+      </c>
+      <c r="E38" s="49" t="s">
+        <v>215</v>
+      </c>
+      <c r="F38" s="49" t="s">
         <v>127</v>
       </c>
-      <c r="C38" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="D38" s="49" t="s">
-        <v>128</v>
-      </c>
-      <c r="E38" s="49" t="s">
-        <v>254</v>
-      </c>
-      <c r="F38" s="49" t="s">
-        <v>129</v>
-      </c>
       <c r="G38" s="49" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="272" x14ac:dyDescent="0.2">
       <c r="A39" s="22" t="s">
-        <v>222</v>
+        <v>264</v>
       </c>
       <c r="B39" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="C39" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="D39" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="C39" s="23" t="s">
+      <c r="E39" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="F39" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="D39" s="25" t="s">
+      <c r="G39" s="25" t="s">
         <v>132</v>
-      </c>
-      <c r="E39" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="F39" s="26" t="s">
-        <v>133</v>
-      </c>
-      <c r="G39" s="25" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="272" x14ac:dyDescent="0.2">
       <c r="A40" s="22" t="s">
-        <v>223</v>
+        <v>265</v>
       </c>
       <c r="B40" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="D40" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="E40" s="25" t="s">
+        <v>134</v>
+      </c>
+      <c r="F40" s="26" t="s">
         <v>135</v>
       </c>
-      <c r="C40" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="D40" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="E40" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="F40" s="26" t="s">
-        <v>137</v>
-      </c>
       <c r="G40" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="272" x14ac:dyDescent="0.2">
       <c r="A41" s="22" t="s">
-        <v>224</v>
+        <v>266</v>
       </c>
       <c r="B41" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="C41" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="D41" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="E41" s="25" t="s">
+        <v>137</v>
+      </c>
+      <c r="F41" s="26" t="s">
         <v>138</v>
       </c>
-      <c r="C41" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="D41" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="E41" s="25" t="s">
-        <v>139</v>
-      </c>
-      <c r="F41" s="26" t="s">
-        <v>140</v>
-      </c>
       <c r="G41" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="272" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
-        <v>225</v>
+        <v>267</v>
       </c>
       <c r="B42" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="D42" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="E42" s="25" t="s">
+        <v>140</v>
+      </c>
+      <c r="F42" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="C42" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="D42" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="E42" s="25" t="s">
-        <v>142</v>
-      </c>
-      <c r="F42" s="26" t="s">
-        <v>143</v>
-      </c>
       <c r="G42" s="25" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A43" s="38" t="s">
-        <v>226</v>
+        <v>268</v>
       </c>
       <c r="B43" s="38" t="s">
+        <v>142</v>
+      </c>
+      <c r="C43" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="D43" s="46" t="s">
         <v>144</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="E43" s="46" t="s">
+        <v>216</v>
+      </c>
+      <c r="F43" s="41" t="s">
         <v>145</v>
-      </c>
-      <c r="D43" s="46" t="s">
-        <v>146</v>
-      </c>
-      <c r="E43" s="46" t="s">
-        <v>255</v>
-      </c>
-      <c r="F43" s="41" t="s">
-        <v>147</v>
       </c>
       <c r="G43" s="44"/>
     </row>
     <row r="44" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A44" s="38" t="s">
-        <v>227</v>
+        <v>269</v>
       </c>
       <c r="B44" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="C44" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="D44" s="46" t="s">
+        <v>147</v>
+      </c>
+      <c r="E44" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="F44" s="41" t="s">
         <v>148</v>
-      </c>
-      <c r="C44" s="39" t="s">
-        <v>145</v>
-      </c>
-      <c r="D44" s="46" t="s">
-        <v>149</v>
-      </c>
-      <c r="E44" s="46" t="s">
-        <v>256</v>
-      </c>
-      <c r="F44" s="41" t="s">
-        <v>150</v>
       </c>
       <c r="G44" s="44"/>
     </row>
     <row r="45" spans="1:7" ht="112" x14ac:dyDescent="0.2">
       <c r="A45" s="22" t="s">
-        <v>228</v>
+        <v>270</v>
       </c>
       <c r="B45" s="22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C45" s="50" t="s">
         <v>48</v>
       </c>
       <c r="D45" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E45" s="25" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F45" s="26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G45" s="36"/>
     </row>
     <row r="46" spans="1:7" ht="128" x14ac:dyDescent="0.2">
       <c r="A46" s="22" t="s">
-        <v>229</v>
+        <v>271</v>
       </c>
       <c r="B46" s="22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C46" s="50" t="s">
         <v>48</v>
       </c>
       <c r="D46" s="25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F46" s="26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="G46" s="36"/>
     </row>
     <row r="47" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A47" s="51" t="s">
-        <v>226</v>
+        <v>272</v>
       </c>
       <c r="B47" s="51" t="s">
+        <v>155</v>
+      </c>
+      <c r="C47" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="D47" s="46" t="s">
         <v>157</v>
       </c>
-      <c r="C47" s="52" t="s">
+      <c r="E47" s="46" t="s">
+        <v>218</v>
+      </c>
+      <c r="F47" s="41" t="s">
         <v>158</v>
-      </c>
-      <c r="D47" s="46" t="s">
-        <v>159</v>
-      </c>
-      <c r="E47" s="46" t="s">
-        <v>257</v>
-      </c>
-      <c r="F47" s="41" t="s">
-        <v>160</v>
       </c>
       <c r="G47" s="53"/>
     </row>
     <row r="48" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A48" s="51" t="s">
-        <v>227</v>
+        <v>273</v>
       </c>
       <c r="B48" s="51" t="s">
+        <v>159</v>
+      </c>
+      <c r="C48" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="D48" s="46" t="s">
+        <v>160</v>
+      </c>
+      <c r="E48" s="46" t="s">
+        <v>219</v>
+      </c>
+      <c r="F48" s="41" t="s">
         <v>161</v>
-      </c>
-      <c r="C48" s="52" t="s">
-        <v>158</v>
-      </c>
-      <c r="D48" s="46" t="s">
-        <v>162</v>
-      </c>
-      <c r="E48" s="46" t="s">
-        <v>258</v>
-      </c>
-      <c r="F48" s="41" t="s">
-        <v>163</v>
       </c>
       <c r="G48" s="53"/>
     </row>
     <row r="49" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A49" s="51" t="s">
-        <v>226</v>
+        <v>274</v>
       </c>
       <c r="B49" s="51" t="s">
+        <v>162</v>
+      </c>
+      <c r="C49" s="52" t="s">
+        <v>163</v>
+      </c>
+      <c r="D49" s="46" t="s">
         <v>164</v>
       </c>
-      <c r="C49" s="52" t="s">
+      <c r="E49" s="46" t="s">
+        <v>220</v>
+      </c>
+      <c r="F49" s="41" t="s">
         <v>165</v>
-      </c>
-      <c r="D49" s="46" t="s">
-        <v>166</v>
-      </c>
-      <c r="E49" s="46" t="s">
-        <v>259</v>
-      </c>
-      <c r="F49" s="41" t="s">
-        <v>167</v>
       </c>
       <c r="G49" s="53"/>
     </row>
     <row r="50" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A50" s="51" t="s">
-        <v>227</v>
+        <v>275</v>
       </c>
       <c r="B50" s="51" t="s">
+        <v>166</v>
+      </c>
+      <c r="C50" s="52" t="s">
+        <v>163</v>
+      </c>
+      <c r="D50" s="46" t="s">
+        <v>167</v>
+      </c>
+      <c r="E50" s="46" t="s">
+        <v>221</v>
+      </c>
+      <c r="F50" s="41" t="s">
         <v>168</v>
-      </c>
-      <c r="C50" s="52" t="s">
-        <v>165</v>
-      </c>
-      <c r="D50" s="46" t="s">
-        <v>169</v>
-      </c>
-      <c r="E50" s="46" t="s">
-        <v>260</v>
-      </c>
-      <c r="F50" s="41" t="s">
-        <v>170</v>
       </c>
       <c r="G50" s="53"/>
     </row>
     <row r="51" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A51" s="51" t="s">
-        <v>226</v>
+        <v>276</v>
       </c>
       <c r="B51" s="51" t="s">
+        <v>169</v>
+      </c>
+      <c r="C51" s="52" t="s">
+        <v>170</v>
+      </c>
+      <c r="D51" s="46" t="s">
         <v>171</v>
       </c>
-      <c r="C51" s="52" t="s">
+      <c r="E51" s="46" t="s">
+        <v>222</v>
+      </c>
+      <c r="F51" s="41" t="s">
         <v>172</v>
-      </c>
-      <c r="D51" s="46" t="s">
-        <v>173</v>
-      </c>
-      <c r="E51" s="46" t="s">
-        <v>261</v>
-      </c>
-      <c r="F51" s="41" t="s">
-        <v>174</v>
       </c>
       <c r="G51" s="53"/>
     </row>
     <row r="52" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A52" s="51" t="s">
-        <v>227</v>
+        <v>277</v>
       </c>
       <c r="B52" s="51" t="s">
+        <v>173</v>
+      </c>
+      <c r="C52" s="52" t="s">
+        <v>170</v>
+      </c>
+      <c r="D52" s="46" t="s">
+        <v>174</v>
+      </c>
+      <c r="E52" s="46" t="s">
+        <v>223</v>
+      </c>
+      <c r="F52" s="41" t="s">
         <v>175</v>
-      </c>
-      <c r="C52" s="52" t="s">
-        <v>172</v>
-      </c>
-      <c r="D52" s="46" t="s">
-        <v>176</v>
-      </c>
-      <c r="E52" s="46" t="s">
-        <v>262</v>
-      </c>
-      <c r="F52" s="41" t="s">
-        <v>177</v>
       </c>
       <c r="G52" s="53"/>
     </row>
     <row r="53" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A53" s="51" t="s">
-        <v>226</v>
+        <v>278</v>
       </c>
       <c r="B53" s="51" t="s">
+        <v>176</v>
+      </c>
+      <c r="C53" s="52" t="s">
+        <v>177</v>
+      </c>
+      <c r="D53" s="46" t="s">
         <v>178</v>
       </c>
-      <c r="C53" s="52" t="s">
+      <c r="E53" s="46" t="s">
+        <v>224</v>
+      </c>
+      <c r="F53" s="41" t="s">
         <v>179</v>
-      </c>
-      <c r="D53" s="46" t="s">
-        <v>180</v>
-      </c>
-      <c r="E53" s="46" t="s">
-        <v>263</v>
-      </c>
-      <c r="F53" s="41" t="s">
-        <v>181</v>
       </c>
       <c r="G53" s="53"/>
     </row>
     <row r="54" spans="1:7" ht="160" x14ac:dyDescent="0.2">
       <c r="A54" s="51" t="s">
-        <v>227</v>
+        <v>279</v>
       </c>
       <c r="B54" s="51" t="s">
+        <v>180</v>
+      </c>
+      <c r="C54" s="52" t="s">
+        <v>177</v>
+      </c>
+      <c r="D54" s="46" t="s">
+        <v>181</v>
+      </c>
+      <c r="E54" s="46" t="s">
+        <v>225</v>
+      </c>
+      <c r="F54" s="41" t="s">
         <v>182</v>
-      </c>
-      <c r="C54" s="52" t="s">
-        <v>179</v>
-      </c>
-      <c r="D54" s="46" t="s">
-        <v>183</v>
-      </c>
-      <c r="E54" s="46" t="s">
-        <v>264</v>
-      </c>
-      <c r="F54" s="41" t="s">
-        <v>184</v>
       </c>
       <c r="G54" s="53"/>
     </row>
     <row r="55" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A55" s="51" t="s">
+        <v>280</v>
+      </c>
+      <c r="B55" s="51" t="s">
+        <v>183</v>
+      </c>
+      <c r="C55" s="52" t="s">
+        <v>184</v>
+      </c>
+      <c r="D55" s="46" t="s">
+        <v>185</v>
+      </c>
+      <c r="E55" s="46" t="s">
         <v>226</v>
       </c>
-      <c r="B55" s="51" t="s">
-        <v>185</v>
-      </c>
-      <c r="C55" s="52" t="s">
+      <c r="F55" s="41" t="s">
         <v>186</v>
-      </c>
-      <c r="D55" s="46" t="s">
-        <v>187</v>
-      </c>
-      <c r="E55" s="46" t="s">
-        <v>265</v>
-      </c>
-      <c r="F55" s="41" t="s">
-        <v>188</v>
       </c>
       <c r="G55" s="53"/>
     </row>
     <row r="56" spans="1:7" ht="144" x14ac:dyDescent="0.2">
       <c r="A56" s="51" t="s">
+        <v>281</v>
+      </c>
+      <c r="B56" s="51" t="s">
+        <v>187</v>
+      </c>
+      <c r="C56" s="52" t="s">
+        <v>184</v>
+      </c>
+      <c r="D56" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="E56" s="46" t="s">
         <v>227</v>
       </c>
-      <c r="B56" s="51" t="s">
+      <c r="F56" s="41" t="s">
         <v>189</v>
-      </c>
-      <c r="C56" s="52" t="s">
-        <v>186</v>
-      </c>
-      <c r="D56" s="46" t="s">
-        <v>190</v>
-      </c>
-      <c r="E56" s="46" t="s">
-        <v>266</v>
-      </c>
-      <c r="F56" s="41" t="s">
-        <v>191</v>
       </c>
       <c r="G56" s="53"/>
     </row>
@@ -3266,26 +3293,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3b0c4c8b-09b7-4186-9978-0ad6f7aa3547">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="42387920-875b-4eae-aa9b-06edaadfbbd9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B083713AC7608747A82F5A763B7281ED" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="427dd16ae52d8d155578e7a775f968a8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3b0c4c8b-09b7-4186-9978-0ad6f7aa3547" xmlns:ns3="42387920-875b-4eae-aa9b-06edaadfbbd9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="154d5f4f1df4d06a6441f4dc4f97264b" ns2:_="" ns3:_="">
     <xsd:import namespace="3b0c4c8b-09b7-4186-9978-0ad6f7aa3547"/>
@@ -3508,10 +3515,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3b0c4c8b-09b7-4186-9978-0ad6f7aa3547">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="42387920-875b-4eae-aa9b-06edaadfbbd9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3CD4AA4-09C8-4CFA-BB33-8F852CC5F422}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C75314D-5D32-4004-AEB1-819C7303AD9A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3b0c4c8b-09b7-4186-9978-0ad6f7aa3547"/>
+    <ds:schemaRef ds:uri="42387920-875b-4eae-aa9b-06edaadfbbd9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3528,20 +3566,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8C75314D-5D32-4004-AEB1-819C7303AD9A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D3CD4AA4-09C8-4CFA-BB33-8F852CC5F422}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="3b0c4c8b-09b7-4186-9978-0ad6f7aa3547"/>
-    <ds:schemaRef ds:uri="42387920-875b-4eae-aa9b-06edaadfbbd9"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update data migration source datasheet
</commit_message>
<xml_diff>
--- a/cms/metrics_documentation/data_migration/source_data/metrics_definitions_migration_edit.xlsx
+++ b/cms/metrics_documentation/data_migration/source_data/metrics_definitions_migration_edit.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="288">
   <si>
     <t>Title</t>
   </si>
@@ -582,6 +582,9 @@
 A change from a number greater than 0 to 0 will be displayed as -100% i.e. a 100% decrease</t>
   </si>
   <si>
+    <t>COVID-19 deaths ONS by day</t>
+  </si>
+  <si>
     <t>COVID-19_deaths_ONSByDay</t>
   </si>
   <si>
@@ -690,7 +693,7 @@
     </r>
   </si>
   <si>
-    <t>COVID-19 deaths ONS by day</t>
+    <t>COVID-19 deaths ONS rolling mean</t>
   </si>
   <si>
     <t>COVID-19_deaths_ONSRollingMean</t>
@@ -2184,17 +2187,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2222,10 +2225,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2473,12 +2476,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -2765,7 +2768,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2793,10 +2796,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -3056,7 +3059,7 @@
     <col min="1" max="1" width="40" style="1" customWidth="1"/>
     <col min="2" max="2" width="50.1719" style="1" customWidth="1"/>
     <col min="3" max="3" width="62.6719" style="1" customWidth="1"/>
-    <col min="4" max="4" width="108.547" style="1" customWidth="1"/>
+    <col min="4" max="4" width="108.5" style="1" customWidth="1"/>
     <col min="5" max="5" width="106.172" style="1" customWidth="1"/>
     <col min="6" max="6" width="91.6719" style="1" customWidth="1"/>
     <col min="7" max="7" width="47" style="1" customWidth="1"/>
@@ -3291,127 +3294,127 @@
     </row>
     <row r="11" ht="202.75" customHeight="1">
       <c r="A11" t="s" s="9">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B11" t="s" s="9">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C11" t="s" s="9">
         <v>50</v>
       </c>
       <c r="D11" t="s" s="9">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s" s="9">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="F11" t="s" s="10">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="G11" s="12"/>
     </row>
     <row r="12" ht="244.75" customHeight="1">
       <c r="A12" t="s" s="9">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B12" t="s" s="9">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C12" t="s" s="9">
         <v>50</v>
       </c>
       <c r="D12" t="s" s="9">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E12" t="s" s="9">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="F12" t="s" s="10">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G12" s="12"/>
     </row>
     <row r="13" ht="244.75" customHeight="1">
       <c r="A13" t="s" s="9">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s" s="9">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C13" t="s" s="9">
         <v>50</v>
       </c>
       <c r="D13" t="s" s="9">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s" s="9">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F13" t="s" s="10">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G13" s="12"/>
     </row>
     <row r="14" ht="138.5" customHeight="1">
       <c r="A14" t="s" s="13">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s" s="13">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C14" t="s" s="13">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D14" t="s" s="13">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E14" t="s" s="13">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F14" t="s" s="14">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G14" s="15"/>
     </row>
     <row r="15" ht="201" customHeight="1">
       <c r="A15" t="s" s="13">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s" s="13">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C15" t="s" s="13">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D15" t="s" s="13">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="E15" t="s" s="13">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="F15" t="s" s="14">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G15" s="15"/>
     </row>
     <row r="16" ht="208.75" customHeight="1">
       <c r="A16" t="s" s="13">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B16" t="s" s="13">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C16" t="s" s="13">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D16" t="s" s="13">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E16" t="s" s="13">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="F16" t="s" s="14">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="G16" t="s" s="14">
         <v>59</v>
@@ -3419,64 +3422,64 @@
     </row>
     <row r="17" ht="176" customHeight="1">
       <c r="A17" t="s" s="13">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B17" t="s" s="13">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C17" t="s" s="13">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D17" t="s" s="13">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E17" t="s" s="13">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="F17" t="s" s="14">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G17" s="16"/>
     </row>
     <row r="18" ht="192" customHeight="1">
       <c r="A18" t="s" s="13">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B18" t="s" s="13">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s" s="13">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D18" t="s" s="13">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E18" t="s" s="13">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F18" t="s" s="14">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G18" s="16"/>
     </row>
     <row r="19" ht="192" customHeight="1">
       <c r="A19" t="s" s="13">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B19" t="s" s="13">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C19" t="s" s="13">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D19" t="s" s="13">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E19" t="s" s="13">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="F19" t="s" s="14">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="G19" t="s" s="17">
         <v>59</v>
@@ -3484,818 +3487,818 @@
     </row>
     <row r="20" ht="156.5" customHeight="1">
       <c r="A20" t="s" s="13">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B20" t="s" s="13">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C20" t="s" s="13">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D20" t="s" s="13">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E20" t="s" s="13">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F20" t="s" s="14">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G20" s="18"/>
     </row>
     <row r="21" ht="176" customHeight="1">
       <c r="A21" t="s" s="13">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B21" t="s" s="13">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C21" t="s" s="13">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D21" t="s" s="13">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="E21" t="s" s="13">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F21" t="s" s="14">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G21" s="15"/>
     </row>
     <row r="22" ht="96" customHeight="1">
       <c r="A22" t="s" s="13">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B22" t="s" s="13">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C22" t="s" s="13">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D22" t="s" s="13">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E22" t="s" s="13">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F22" t="s" s="14">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G22" s="15"/>
     </row>
     <row r="23" ht="128" customHeight="1">
       <c r="A23" t="s" s="19">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B23" t="s" s="19">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C23" t="s" s="19">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D23" t="s" s="19">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E23" t="s" s="19">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F23" t="s" s="20">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G23" t="s" s="20">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="24" ht="128" customHeight="1">
       <c r="A24" t="s" s="19">
+        <v>120</v>
+      </c>
+      <c r="B24" t="s" s="19">
+        <v>121</v>
+      </c>
+      <c r="C24" t="s" s="19">
+        <v>115</v>
+      </c>
+      <c r="D24" t="s" s="19">
+        <v>122</v>
+      </c>
+      <c r="E24" t="s" s="21">
+        <v>123</v>
+      </c>
+      <c r="F24" t="s" s="20">
+        <v>124</v>
+      </c>
+      <c r="G24" t="s" s="20">
         <v>119</v>
-      </c>
-      <c r="B24" t="s" s="19">
-        <v>120</v>
-      </c>
-      <c r="C24" t="s" s="19">
-        <v>114</v>
-      </c>
-      <c r="D24" t="s" s="19">
-        <v>121</v>
-      </c>
-      <c r="E24" t="s" s="21">
-        <v>122</v>
-      </c>
-      <c r="F24" t="s" s="20">
-        <v>123</v>
-      </c>
-      <c r="G24" t="s" s="20">
-        <v>118</v>
       </c>
     </row>
     <row r="25" ht="160" customHeight="1">
       <c r="A25" t="s" s="19">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B25" t="s" s="19">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C25" t="s" s="19">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D25" t="s" s="22">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="E25" t="s" s="23">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F25" t="s" s="20">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="G25" t="s" s="20">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" ht="160" customHeight="1">
       <c r="A26" t="s" s="19">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B26" t="s" s="19">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C26" t="s" s="19">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D26" t="s" s="19">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E26" t="s" s="19">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F26" t="s" s="20">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G26" t="s" s="20">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" ht="112" customHeight="1">
       <c r="A27" t="s" s="19">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B27" t="s" s="19">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C27" t="s" s="19">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D27" t="s" s="19">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E27" t="s" s="19">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F27" t="s" s="20">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G27" t="s" s="20">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="28" ht="144" customHeight="1">
       <c r="A28" t="s" s="19">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B28" t="s" s="19">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C28" t="s" s="19">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D28" t="s" s="19">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E28" t="s" s="19">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F28" t="s" s="20">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="G28" t="s" s="20">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" ht="176" customHeight="1">
       <c r="A29" t="s" s="24">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B29" t="s" s="24">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C29" t="s" s="24">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D29" t="s" s="24">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="E29" t="s" s="24">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="F29" t="s" s="25">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="G29" t="s" s="25">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="30" ht="192" customHeight="1">
       <c r="A30" t="s" s="24">
+        <v>152</v>
+      </c>
+      <c r="B30" t="s" s="24">
+        <v>153</v>
+      </c>
+      <c r="C30" t="s" s="24">
+        <v>148</v>
+      </c>
+      <c r="D30" t="s" s="24">
+        <v>154</v>
+      </c>
+      <c r="E30" t="s" s="24">
+        <v>154</v>
+      </c>
+      <c r="F30" t="s" s="25">
+        <v>155</v>
+      </c>
+      <c r="G30" t="s" s="25">
         <v>151</v>
-      </c>
-      <c r="B30" t="s" s="24">
-        <v>152</v>
-      </c>
-      <c r="C30" t="s" s="24">
-        <v>147</v>
-      </c>
-      <c r="D30" t="s" s="24">
-        <v>153</v>
-      </c>
-      <c r="E30" t="s" s="24">
-        <v>153</v>
-      </c>
-      <c r="F30" t="s" s="25">
-        <v>154</v>
-      </c>
-      <c r="G30" t="s" s="25">
-        <v>150</v>
       </c>
     </row>
     <row r="31" ht="176" customHeight="1">
       <c r="A31" t="s" s="24">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B31" t="s" s="24">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="C31" t="s" s="24">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D31" t="s" s="24">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E31" t="s" s="24">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F31" t="s" s="25">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="G31" t="s" s="25">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="32" ht="192" customHeight="1">
       <c r="A32" t="s" s="24">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B32" t="s" s="24">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C32" t="s" s="24">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D32" t="s" s="24">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="E32" t="s" s="24">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="F32" t="s" s="25">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="G32" t="s" s="25">
-        <v>150</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" ht="176" customHeight="1">
       <c r="A33" t="s" s="24">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B33" t="s" s="24">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C33" t="s" s="24">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D33" t="s" s="24">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="E33" t="s" s="24">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="F33" t="s" s="25">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="G33" t="s" s="25">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" ht="192" customHeight="1">
       <c r="A34" t="s" s="24">
+        <v>171</v>
+      </c>
+      <c r="B34" t="s" s="24">
+        <v>172</v>
+      </c>
+      <c r="C34" t="s" s="24">
+        <v>148</v>
+      </c>
+      <c r="D34" t="s" s="24">
+        <v>173</v>
+      </c>
+      <c r="E34" t="s" s="24">
+        <v>173</v>
+      </c>
+      <c r="F34" t="s" s="25">
+        <v>174</v>
+      </c>
+      <c r="G34" t="s" s="25">
         <v>170</v>
-      </c>
-      <c r="B34" t="s" s="24">
-        <v>171</v>
-      </c>
-      <c r="C34" t="s" s="24">
-        <v>147</v>
-      </c>
-      <c r="D34" t="s" s="24">
-        <v>172</v>
-      </c>
-      <c r="E34" t="s" s="24">
-        <v>172</v>
-      </c>
-      <c r="F34" t="s" s="25">
-        <v>173</v>
-      </c>
-      <c r="G34" t="s" s="25">
-        <v>169</v>
       </c>
     </row>
     <row r="35" ht="176" customHeight="1">
       <c r="A35" t="s" s="24">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B35" t="s" s="24">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C35" t="s" s="24">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D35" t="s" s="24">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E35" t="s" s="24">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="F35" t="s" s="25">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="G35" t="s" s="25">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" ht="192" customHeight="1">
       <c r="A36" t="s" s="24">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B36" t="s" s="24">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C36" t="s" s="24">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D36" t="s" s="24">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="E36" t="s" s="24">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="F36" t="s" s="25">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G36" t="s" s="25">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" ht="176" customHeight="1">
       <c r="A37" t="s" s="24">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B37" t="s" s="24">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C37" t="s" s="24">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="D37" t="s" s="24">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E37" t="s" s="24">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="F37" t="s" s="25">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="G37" t="s" s="25">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="38" ht="192" customHeight="1">
       <c r="A38" t="s" s="24">
+        <v>191</v>
+      </c>
+      <c r="B38" t="s" s="24">
+        <v>192</v>
+      </c>
+      <c r="C38" t="s" s="24">
+        <v>148</v>
+      </c>
+      <c r="D38" t="s" s="24">
+        <v>193</v>
+      </c>
+      <c r="E38" t="s" s="24">
+        <v>194</v>
+      </c>
+      <c r="F38" t="s" s="25">
+        <v>195</v>
+      </c>
+      <c r="G38" t="s" s="25">
         <v>190</v>
-      </c>
-      <c r="B38" t="s" s="24">
-        <v>191</v>
-      </c>
-      <c r="C38" t="s" s="24">
-        <v>147</v>
-      </c>
-      <c r="D38" t="s" s="24">
-        <v>192</v>
-      </c>
-      <c r="E38" t="s" s="24">
-        <v>193</v>
-      </c>
-      <c r="F38" t="s" s="25">
-        <v>194</v>
-      </c>
-      <c r="G38" t="s" s="25">
-        <v>189</v>
       </c>
     </row>
     <row r="39" ht="272" customHeight="1">
       <c r="A39" t="s" s="13">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B39" t="s" s="13">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="C39" t="s" s="13">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D39" t="s" s="13">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E39" t="s" s="13">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F39" t="s" s="14">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G39" t="s" s="14">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="40" ht="272" customHeight="1">
       <c r="A40" t="s" s="13">
+        <v>202</v>
+      </c>
+      <c r="B40" t="s" s="13">
+        <v>203</v>
+      </c>
+      <c r="C40" t="s" s="13">
+        <v>198</v>
+      </c>
+      <c r="D40" t="s" s="13">
+        <v>204</v>
+      </c>
+      <c r="E40" t="s" s="13">
+        <v>204</v>
+      </c>
+      <c r="F40" t="s" s="14">
+        <v>205</v>
+      </c>
+      <c r="G40" t="s" s="14">
         <v>201</v>
-      </c>
-      <c r="B40" t="s" s="13">
-        <v>202</v>
-      </c>
-      <c r="C40" t="s" s="13">
-        <v>197</v>
-      </c>
-      <c r="D40" t="s" s="13">
-        <v>203</v>
-      </c>
-      <c r="E40" t="s" s="13">
-        <v>203</v>
-      </c>
-      <c r="F40" t="s" s="14">
-        <v>204</v>
-      </c>
-      <c r="G40" t="s" s="14">
-        <v>200</v>
       </c>
     </row>
     <row r="41" ht="272" customHeight="1">
       <c r="A41" t="s" s="13">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B41" t="s" s="13">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="C41" t="s" s="13">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D41" t="s" s="13">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="E41" t="s" s="13">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="F41" t="s" s="14">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="G41" t="s" s="14">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42" ht="272" customHeight="1">
       <c r="A42" t="s" s="13">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B42" t="s" s="13">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C42" t="s" s="13">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D42" t="s" s="13">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E42" t="s" s="13">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F42" t="s" s="14">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G42" t="s" s="14">
-        <v>200</v>
+        <v>201</v>
       </c>
     </row>
     <row r="43" ht="160" customHeight="1">
       <c r="A43" t="s" s="19">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B43" t="s" s="19">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C43" t="s" s="19">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D43" t="s" s="19">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="E43" t="s" s="19">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F43" t="s" s="20">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G43" s="26"/>
     </row>
     <row r="44" ht="160" customHeight="1">
       <c r="A44" t="s" s="19">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B44" t="s" s="19">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C44" t="s" s="19">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="D44" t="s" s="19">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E44" t="s" s="19">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F44" t="s" s="20">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="G44" s="26"/>
     </row>
     <row r="45" ht="112" customHeight="1">
       <c r="A45" t="s" s="13">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B45" t="s" s="13">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C45" t="s" s="13">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D45" t="s" s="13">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E45" t="s" s="13">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F45" t="s" s="14">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G45" s="15"/>
     </row>
     <row r="46" ht="128" customHeight="1">
       <c r="A46" t="s" s="13">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="B46" t="s" s="13">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C46" t="s" s="13">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D46" t="s" s="13">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="E46" t="s" s="13">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F46" t="s" s="14">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G46" s="15"/>
     </row>
     <row r="47" ht="160" customHeight="1">
       <c r="A47" t="s" s="27">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B47" t="s" s="27">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="C47" t="s" s="27">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D47" t="s" s="19">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E47" t="s" s="19">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F47" t="s" s="20">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="G47" s="28"/>
     </row>
     <row r="48" ht="160" customHeight="1">
       <c r="A48" t="s" s="27">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B48" t="s" s="27">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C48" t="s" s="27">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="D48" t="s" s="19">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E48" t="s" s="19">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="F48" t="s" s="20">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="G48" s="28"/>
     </row>
     <row r="49" ht="144" customHeight="1">
       <c r="A49" t="s" s="27">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B49" t="s" s="27">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="C49" t="s" s="27">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D49" t="s" s="19">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E49" t="s" s="19">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="F49" t="s" s="20">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="G49" s="28"/>
     </row>
     <row r="50" ht="144" customHeight="1">
       <c r="A50" t="s" s="27">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B50" t="s" s="27">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C50" t="s" s="27">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="D50" t="s" s="19">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="E50" t="s" s="19">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="F50" t="s" s="20">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="G50" s="28"/>
     </row>
     <row r="51" ht="160" customHeight="1">
       <c r="A51" t="s" s="27">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B51" t="s" s="27">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C51" t="s" s="27">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D51" t="s" s="19">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E51" t="s" s="19">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F51" t="s" s="20">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="G51" s="28"/>
     </row>
     <row r="52" ht="160" customHeight="1">
       <c r="A52" t="s" s="27">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B52" t="s" s="27">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="C52" t="s" s="27">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D52" t="s" s="19">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E52" t="s" s="19">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F52" t="s" s="20">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G52" s="28"/>
     </row>
     <row r="53" ht="160" customHeight="1">
       <c r="A53" t="s" s="27">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B53" t="s" s="27">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C53" t="s" s="27">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D53" t="s" s="19">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="E53" t="s" s="19">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F53" t="s" s="20">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="G53" s="28"/>
     </row>
     <row r="54" ht="160" customHeight="1">
       <c r="A54" t="s" s="27">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B54" t="s" s="27">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C54" t="s" s="27">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="D54" t="s" s="19">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="E54" t="s" s="19">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="F54" t="s" s="20">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="G54" s="28"/>
     </row>
     <row r="55" ht="144" customHeight="1">
       <c r="A55" t="s" s="27">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B55" t="s" s="27">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C55" t="s" s="27">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D55" t="s" s="19">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E55" t="s" s="19">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="F55" t="s" s="20">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="G55" s="28"/>
     </row>
     <row r="56" ht="144" customHeight="1">
       <c r="A56" t="s" s="27">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B56" t="s" s="27">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C56" t="s" s="27">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="D56" t="s" s="19">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E56" t="s" s="19">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="F56" t="s" s="20">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="G56" s="28"/>
     </row>

</xml_diff>